<commit_message>
Update maize validation and start cleaning up maize.xml file
</commit_message>
<xml_diff>
--- a/Tests/Maize/Ciampitti Yield Components.xlsx
+++ b/Tests/Maize/Ciampitti Yield Components.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr hidePivotFieldList="1" showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="12" windowWidth="12120" windowHeight="6456" activeTab="1"/>
+    <workbookView xWindow="192" yWindow="12" windowWidth="12120" windowHeight="5304" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="31">
   <si>
     <t>Location</t>
   </si>
@@ -87,6 +87,33 @@
   <si>
     <t>Sum of GrainSize</t>
   </si>
+  <si>
+    <t>Lincoln12</t>
+  </si>
+  <si>
+    <t>Dry_000N</t>
+  </si>
+  <si>
+    <t>Dry_075N</t>
+  </si>
+  <si>
+    <t>Dry_250N</t>
+  </si>
+  <si>
+    <t>Irrig_000N</t>
+  </si>
+  <si>
+    <t>Irrig_075N</t>
+  </si>
+  <si>
+    <t>Irrig_250N</t>
+  </si>
+  <si>
+    <t>SilkCobWt</t>
+  </si>
+  <si>
+    <t>SilkEarPerm2</t>
+  </si>
 </sst>
 </file>
 
@@ -121,13 +148,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,6 +192,15 @@
       <c:pivotFmt>
         <c:idx val="5"/>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -320,24 +357,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="109321216"/>
-        <c:axId val="114053888"/>
+        <c:axId val="99736576"/>
+        <c:axId val="111948544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="109321216"/>
+        <c:axId val="99736576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114053888"/>
+        <c:crossAx val="111948544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114053888"/>
+        <c:axId val="111948544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -345,20 +382,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109321216"/>
+        <c:crossAx val="99736576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -380,43 +416,35 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.12386014248218973"/>
+                  <c:y val="8.7168356154894129E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr>
+                      <a:solidFill>
+                        <a:srgbClr val="0070C0"/>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$G$4:$G$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>644</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>684</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>801</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>598</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>554</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>532</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>438</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>527</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>499</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$I$4:$I$12</c:f>
               <c:numCache>
@@ -448,6 +476,1260 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>25.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$4:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>644</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.17203201162354706"/>
+                  <c:y val="-0.11490020858829597"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr>
+                      <a:solidFill>
+                        <a:srgbClr val="C00000"/>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$13:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$13:$J$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>661</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>481</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>475</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.5736548556430448E-2"/>
+                  <c:y val="0.39402098198135788"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr>
+                      <a:solidFill>
+                        <a:srgbClr val="00B050"/>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$22:$I$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>21.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.100000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$22:$J$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>622</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>566</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.1939536464191976"/>
+                  <c:y val="0.38211451574418298"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:txPr>
+                <a:bodyPr/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr>
+                      <a:solidFill>
+                        <a:srgbClr val="7030A0"/>
+                      </a:solidFill>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$31:$I$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$31:$J$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>678</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>563</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>467</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="113863296"/>
+        <c:axId val="113873280"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="113863296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113873280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="113873280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113863296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-AU"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GPEar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.2436916315693097"/>
+                  <c:y val="-8.2496521519147464E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$4:$I$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>25.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>21.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>16.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$4:$J$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>644</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>661</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>481</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>622</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>566</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>597</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>678</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>563</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>467</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.24460891032031848"/>
+                  <c:y val="0.45959744489770105"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$22:$I$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>21.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$22:$J$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>622</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>566</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>678</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>563</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>467</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$19:$P$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$19:$Q$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>179.54669066930211</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>334.1802256933596</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>398.83809198154268</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>487.6635381918756</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>562.44156085567636</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>687.70322370746237</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$41:$I$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12.941666666666668</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.708333333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.491666666666664</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.175000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.183333333333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$41:$J$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>267.16666666666669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>244.91666666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>398.16666666666669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>437.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>434.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="113892352"/>
+        <c:axId val="114230016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="113892352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="114230016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="114230016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113892352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-AU"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$H$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>33.518518518518519</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.703703703703702</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.886075949367086</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.924050632911392</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.759493670886076</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5961538461538463</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9615384615384617</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3653846153846154</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.407407407407405</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38.703703703703702</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>38.888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.582278481012658</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>38.734177215189874</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>34.050632911392405</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5288461538461537</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.3557692307692308</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.4519230769230771</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31.296296296296294</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29.814814814814813</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.8481012658227849</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18.860759493670884</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22.911392405063289</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.81730769230769229</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.1057692307692308</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.98076923076923073</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>21.851851851851851</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>34.629629629629626</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32.962962962962962</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.177215189873417</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>20.50632911392405</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24.556962025316455</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.7403846153846154</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.9903846153846154</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.9230769230769231</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$4:$J$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>644</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>661</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>481</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>622</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>566</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>597</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>678</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>563</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -463,80 +1745,109 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$13:$G$21</c:f>
+              <c:f>Sheet1!$H$40:$H$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>612</c:v>
+                  <c:v>12.608333333333334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>661</c:v>
+                  <c:v>17.516666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>654</c:v>
+                  <c:v>19.083333333333332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>481</c:v>
+                  <c:v>28.158333333333331</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>548</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>576</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>405</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>556</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>475</c:v>
+                  <c:v>38.43333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>47.358333333333327</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$13:$I$21</c:f>
+              <c:f>Sheet1!$J$40:$J$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.1</c:v>
+                  <c:v>267.16666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.2</c:v>
+                  <c:v>244.91666666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.8</c:v>
+                  <c:v>398.16666666666669</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.899999999999999</c:v>
+                  <c:v>437.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13</c:v>
+                  <c:v>434.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
+        <c:axId val="152588288"/>
+        <c:axId val="136708096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="152588288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="136708096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="136708096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152588288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-AU"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="0"/>
+          <c:order val="0"/>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -544,175 +1855,76 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$22:$G$30</c:f>
+              <c:f>Sheet1!$L$40:$L$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>622</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>687</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>643</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>456</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>566</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>597</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>355</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>459</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>499</c:v>
+                  <c:v>5.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$22:$I$30</c:f>
+              <c:f>Sheet1!$M$40:$M$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>21.2</c:v>
+                  <c:v>2053.2841812839974</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.8</c:v>
+                  <c:v>2666.9280374251107</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.6</c:v>
+                  <c:v>2965.1934863256661</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.5</c:v>
+                  <c:v>4872.3193140456788</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.600000000000001</c:v>
+                  <c:v>5012.0274073398868</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18.100000000000001</c:v>
+                  <c:v>5640.0645645995637</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$G$31:$G$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>545</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>678</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>484</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>561</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>563</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>410</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>461</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>467</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$31:$I$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>17.600000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>25.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>22.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>17.3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16.7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="119622272"/>
-        <c:axId val="119640448"/>
+        <c:axId val="152271104"/>
+        <c:axId val="152269568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119622272"/>
+        <c:axId val="152271104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119640448"/>
+        <c:crossAx val="152269568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119640448"/>
+        <c:axId val="152269568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -720,7 +1932,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119622272"/>
+        <c:crossAx val="152271104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -733,7 +1945,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -778,16 +1990,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -806,13 +2018,103 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Huth, Neil (Agriculture, Toowoomba)" refreshedDate="42047.574480439813" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="36">
   <cacheSource type="worksheet">
-    <worksheetSource ref="B3:I39" sheet="Sheet1"/>
+    <worksheetSource ref="B3:K39" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="Location" numFmtId="0">
@@ -1314,7 +2616,7 @@
             <x v="0"/>
           </reference>
           <reference field="3" count="1" selected="0">
-            <x v="1"/>
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -1326,7 +2628,7 @@
             <x v="0"/>
           </reference>
           <reference field="3" count="1" selected="0">
-            <x v="2"/>
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -1338,7 +2640,7 @@
             <x v="0"/>
           </reference>
           <reference field="3" count="1" selected="0">
-            <x v="0"/>
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -1768,15 +3070,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:I39"/>
+  <dimension ref="B3:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:11">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1793,16 +3095,22 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="2:9">
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1810,7 +3118,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -1819,16 +3127,23 @@
         <v>115.2</v>
       </c>
       <c r="G4">
-        <v>644</v>
+        <v>181</v>
       </c>
       <c r="H4">
-        <v>179</v>
+        <f>G4/D4</f>
+        <v>33.518518518518519</v>
       </c>
       <c r="I4">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="5" spans="2:9">
+      <c r="J4">
+        <v>644</v>
+      </c>
+      <c r="K4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1836,7 +3151,7 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -1845,16 +3160,23 @@
         <v>138.1</v>
       </c>
       <c r="G5">
-        <v>684</v>
+        <v>174</v>
       </c>
       <c r="H5">
-        <v>202</v>
+        <f t="shared" ref="H5:H39" si="0">G5/D5</f>
+        <v>32.222222222222221</v>
       </c>
       <c r="I5">
         <v>24.8</v>
       </c>
-    </row>
-    <row r="6" spans="2:9">
+      <c r="J5">
+        <v>684</v>
+      </c>
+      <c r="K5">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -1862,7 +3184,7 @@
         <v>3</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -1871,16 +3193,23 @@
         <v>142.6</v>
       </c>
       <c r="G6">
-        <v>801</v>
+        <v>155</v>
       </c>
       <c r="H6">
-        <v>178</v>
+        <f t="shared" si="0"/>
+        <v>28.703703703703702</v>
       </c>
       <c r="I6">
         <v>26.3</v>
       </c>
-    </row>
-    <row r="7" spans="2:9">
+      <c r="J6">
+        <v>801</v>
+      </c>
+      <c r="K6">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1888,7 +3217,7 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -1897,16 +3226,23 @@
         <v>108.1</v>
       </c>
       <c r="G7">
-        <v>598</v>
+        <v>165</v>
       </c>
       <c r="H7">
-        <v>181</v>
+        <f t="shared" si="0"/>
+        <v>20.886075949367086</v>
       </c>
       <c r="I7">
         <v>16.100000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="2:9">
+      <c r="J7">
+        <v>598</v>
+      </c>
+      <c r="K7">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -1914,7 +3250,7 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -1923,16 +3259,23 @@
         <v>124.2</v>
       </c>
       <c r="G8">
-        <v>554</v>
+        <v>189</v>
       </c>
       <c r="H8">
-        <v>224</v>
+        <f t="shared" si="0"/>
+        <v>23.924050632911392</v>
       </c>
       <c r="I8">
         <v>23.9</v>
       </c>
-    </row>
-    <row r="9" spans="2:9">
+      <c r="J8">
+        <v>554</v>
+      </c>
+      <c r="K8">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -1940,7 +3283,7 @@
         <v>3</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -1949,16 +3292,23 @@
         <v>145.9</v>
       </c>
       <c r="G9">
-        <v>532</v>
+        <v>164</v>
       </c>
       <c r="H9">
-        <v>274</v>
+        <f t="shared" si="0"/>
+        <v>20.759493670886076</v>
       </c>
       <c r="I9">
         <v>22.3</v>
       </c>
-    </row>
-    <row r="10" spans="2:9">
+      <c r="J9">
+        <v>532</v>
+      </c>
+      <c r="K9">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -1966,7 +3316,7 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -1975,16 +3325,23 @@
         <v>76.8</v>
       </c>
       <c r="G10">
-        <v>438</v>
+        <v>270</v>
       </c>
       <c r="H10">
-        <v>175</v>
+        <f t="shared" si="0"/>
+        <v>2.5961538461538463</v>
       </c>
       <c r="I10">
         <v>15.2</v>
       </c>
-    </row>
-    <row r="11" spans="2:9">
+      <c r="J10">
+        <v>438</v>
+      </c>
+      <c r="K10">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -1992,7 +3349,7 @@
         <v>3</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -2001,16 +3358,23 @@
         <v>102.3</v>
       </c>
       <c r="G11">
-        <v>527</v>
+        <v>308</v>
       </c>
       <c r="H11">
-        <v>194</v>
+        <f t="shared" si="0"/>
+        <v>2.9615384615384617</v>
       </c>
       <c r="I11">
         <v>13.9</v>
       </c>
-    </row>
-    <row r="12" spans="2:9">
+      <c r="J11">
+        <v>527</v>
+      </c>
+      <c r="K11">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
       <c r="B12" t="s">
         <v>2</v>
       </c>
@@ -2018,7 +3382,7 @@
         <v>3</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -2027,16 +3391,23 @@
         <v>105.8</v>
       </c>
       <c r="G12">
-        <v>499</v>
+        <v>246</v>
       </c>
       <c r="H12">
-        <v>212</v>
+        <f t="shared" si="0"/>
+        <v>2.3653846153846154</v>
       </c>
       <c r="I12">
         <v>25.8</v>
       </c>
-    </row>
-    <row r="13" spans="2:9">
+      <c r="J12">
+        <v>499</v>
+      </c>
+      <c r="K12">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -2044,7 +3415,7 @@
         <v>9</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -2053,16 +3424,23 @@
         <v>138.1</v>
       </c>
       <c r="G13">
-        <v>612</v>
+        <v>148</v>
       </c>
       <c r="H13">
-        <v>226</v>
+        <f t="shared" si="0"/>
+        <v>27.407407407407405</v>
       </c>
       <c r="I13">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="2:9">
+      <c r="J13">
+        <v>612</v>
+      </c>
+      <c r="K13">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -2070,7 +3448,7 @@
         <v>9</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -2079,16 +3457,23 @@
         <v>159.30000000000001</v>
       </c>
       <c r="G14">
-        <v>661</v>
+        <v>209</v>
       </c>
       <c r="H14">
-        <v>241</v>
+        <f t="shared" si="0"/>
+        <v>38.703703703703702</v>
       </c>
       <c r="I14">
         <v>31.1</v>
       </c>
-    </row>
-    <row r="15" spans="2:9">
+      <c r="J14">
+        <v>661</v>
+      </c>
+      <c r="K14">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
       <c r="B15" t="s">
         <v>2</v>
       </c>
@@ -2096,7 +3481,7 @@
         <v>9</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -2105,16 +3490,23 @@
         <v>153.30000000000001</v>
       </c>
       <c r="G15">
-        <v>654</v>
+        <v>210</v>
       </c>
       <c r="H15">
-        <v>234</v>
+        <f t="shared" si="0"/>
+        <v>38.888888888888886</v>
       </c>
       <c r="I15">
         <v>31.2</v>
       </c>
-    </row>
-    <row r="16" spans="2:9">
+      <c r="J15">
+        <v>654</v>
+      </c>
+      <c r="K15">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
       <c r="B16" t="s">
         <v>2</v>
       </c>
@@ -2122,7 +3514,7 @@
         <v>9</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
@@ -2131,16 +3523,23 @@
         <v>98.4</v>
       </c>
       <c r="G16">
-        <v>481</v>
+        <v>210</v>
       </c>
       <c r="H16">
-        <v>204</v>
+        <f t="shared" si="0"/>
+        <v>26.582278481012658</v>
       </c>
       <c r="I16">
         <v>16.8</v>
       </c>
-    </row>
-    <row r="17" spans="2:9">
+      <c r="J16">
+        <v>481</v>
+      </c>
+      <c r="K16">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -2148,7 +3547,7 @@
         <v>9</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -2157,16 +3556,23 @@
         <v>126.6</v>
       </c>
       <c r="G17">
-        <v>548</v>
+        <v>306</v>
       </c>
       <c r="H17">
-        <v>231</v>
+        <f t="shared" si="0"/>
+        <v>38.734177215189874</v>
       </c>
       <c r="I17">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="2:9">
+      <c r="J17">
+        <v>548</v>
+      </c>
+      <c r="K17">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -2174,7 +3580,7 @@
         <v>9</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -2183,16 +3589,23 @@
         <v>132.19999999999999</v>
       </c>
       <c r="G18">
-        <v>576</v>
+        <v>269</v>
       </c>
       <c r="H18">
-        <v>229</v>
+        <f t="shared" si="0"/>
+        <v>34.050632911392405</v>
       </c>
       <c r="I18">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="19" spans="2:9">
+      <c r="J18">
+        <v>576</v>
+      </c>
+      <c r="K18">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17">
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -2200,7 +3613,7 @@
         <v>9</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
@@ -2209,16 +3622,30 @@
         <v>87.4</v>
       </c>
       <c r="G19">
-        <v>405</v>
+        <v>263</v>
       </c>
       <c r="H19">
-        <v>216</v>
+        <f t="shared" si="0"/>
+        <v>2.5288461538461537</v>
       </c>
       <c r="I19">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="20" spans="2:9">
+      <c r="J19">
+        <v>405</v>
+      </c>
+      <c r="K19">
+        <v>216</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <f>127.32*P19^0.4959</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -2226,7 +3653,7 @@
         <v>9</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
@@ -2235,16 +3662,30 @@
         <v>101.7</v>
       </c>
       <c r="G20">
-        <v>556</v>
+        <v>349</v>
       </c>
       <c r="H20">
-        <v>183</v>
+        <f t="shared" si="0"/>
+        <v>3.3557692307692308</v>
       </c>
       <c r="I20">
         <v>11.8</v>
       </c>
-    </row>
-    <row r="21" spans="2:9">
+      <c r="J20">
+        <v>556</v>
+      </c>
+      <c r="K20">
+        <v>183</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" ref="Q20:Q25" si="1">127.32*P20^0.4959</f>
+        <v>179.54669066930211</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17">
       <c r="B21" t="s">
         <v>2</v>
       </c>
@@ -2252,7 +3693,7 @@
         <v>9</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -2261,16 +3702,30 @@
         <v>117.5</v>
       </c>
       <c r="G21">
-        <v>475</v>
+        <v>359</v>
       </c>
       <c r="H21">
-        <v>247</v>
+        <f t="shared" si="0"/>
+        <v>3.4519230769230771</v>
       </c>
       <c r="I21">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="2:9">
+      <c r="J21">
+        <v>475</v>
+      </c>
+      <c r="K21">
+        <v>247</v>
+      </c>
+      <c r="P21">
+        <v>7</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="1"/>
+        <v>334.1802256933596</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17">
       <c r="B22" t="s">
         <v>14</v>
       </c>
@@ -2278,7 +3733,7 @@
         <v>15</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E22" t="s">
         <v>6</v>
@@ -2287,16 +3742,30 @@
         <v>107.6</v>
       </c>
       <c r="G22">
-        <v>622</v>
+        <v>169</v>
       </c>
       <c r="H22">
-        <v>173</v>
+        <f t="shared" si="0"/>
+        <v>31.296296296296294</v>
       </c>
       <c r="I22">
         <v>21.2</v>
       </c>
-    </row>
-    <row r="23" spans="2:9">
+      <c r="J22">
+        <v>622</v>
+      </c>
+      <c r="K22">
+        <v>173</v>
+      </c>
+      <c r="P22">
+        <v>10</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="1"/>
+        <v>398.83809198154268</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17">
       <c r="B23" t="s">
         <v>14</v>
       </c>
@@ -2304,7 +3773,7 @@
         <v>15</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E23" t="s">
         <v>7</v>
@@ -2313,16 +3782,30 @@
         <v>145.69999999999999</v>
       </c>
       <c r="G23">
-        <v>687</v>
+        <v>161</v>
       </c>
       <c r="H23">
-        <v>212</v>
+        <f t="shared" si="0"/>
+        <v>29.814814814814813</v>
       </c>
       <c r="I23">
         <v>23.8</v>
       </c>
-    </row>
-    <row r="24" spans="2:9">
+      <c r="J23">
+        <v>687</v>
+      </c>
+      <c r="K23">
+        <v>212</v>
+      </c>
+      <c r="P23">
+        <v>15</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="1"/>
+        <v>487.6635381918756</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17">
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -2330,7 +3813,7 @@
         <v>15</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -2339,16 +3822,30 @@
         <v>143.9</v>
       </c>
       <c r="G24">
-        <v>643</v>
+        <v>144</v>
       </c>
       <c r="H24">
-        <v>224</v>
+        <f t="shared" si="0"/>
+        <v>26.666666666666664</v>
       </c>
       <c r="I24">
         <v>23.6</v>
       </c>
-    </row>
-    <row r="25" spans="2:9">
+      <c r="J24">
+        <v>643</v>
+      </c>
+      <c r="K24">
+        <v>224</v>
+      </c>
+      <c r="P24">
+        <v>20</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="1"/>
+        <v>562.44156085567636</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17">
       <c r="B25" t="s">
         <v>14</v>
       </c>
@@ -2356,7 +3853,7 @@
         <v>15</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E25" t="s">
         <v>6</v>
@@ -2365,16 +3862,30 @@
         <v>80.8</v>
       </c>
       <c r="G25">
-        <v>456</v>
+        <v>62</v>
       </c>
       <c r="H25">
-        <v>177</v>
+        <f t="shared" si="0"/>
+        <v>7.8481012658227849</v>
       </c>
       <c r="I25">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="26" spans="2:9">
+      <c r="J25">
+        <v>456</v>
+      </c>
+      <c r="K25">
+        <v>177</v>
+      </c>
+      <c r="P25">
+        <v>30</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="1"/>
+        <v>687.70322370746237</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17">
       <c r="B26" t="s">
         <v>14</v>
       </c>
@@ -2382,7 +3893,7 @@
         <v>15</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
@@ -2391,16 +3902,23 @@
         <v>122.8</v>
       </c>
       <c r="G26">
-        <v>566</v>
+        <v>149</v>
       </c>
       <c r="H26">
-        <v>217</v>
+        <f t="shared" si="0"/>
+        <v>18.860759493670884</v>
       </c>
       <c r="I26">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="2:9">
+      <c r="J26">
+        <v>566</v>
+      </c>
+      <c r="K26">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17">
       <c r="B27" t="s">
         <v>14</v>
       </c>
@@ -2408,7 +3926,7 @@
         <v>15</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -2417,16 +3935,23 @@
         <v>122</v>
       </c>
       <c r="G27">
-        <v>597</v>
+        <v>181</v>
       </c>
       <c r="H27">
-        <v>204</v>
+        <f t="shared" si="0"/>
+        <v>22.911392405063289</v>
       </c>
       <c r="I27">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="2:9">
+      <c r="J27">
+        <v>597</v>
+      </c>
+      <c r="K27">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17">
       <c r="B28" t="s">
         <v>14</v>
       </c>
@@ -2434,7 +3959,7 @@
         <v>15</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
@@ -2443,16 +3968,23 @@
         <v>72.599999999999994</v>
       </c>
       <c r="G28">
-        <v>355</v>
+        <v>85</v>
       </c>
       <c r="H28">
-        <v>204</v>
+        <f t="shared" si="0"/>
+        <v>0.81730769230769229</v>
       </c>
       <c r="I28">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="29" spans="2:9">
+      <c r="J28">
+        <v>355</v>
+      </c>
+      <c r="K28">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17">
       <c r="B29" t="s">
         <v>14</v>
       </c>
@@ -2460,7 +3992,7 @@
         <v>15</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
@@ -2469,16 +4001,23 @@
         <v>100.1</v>
       </c>
       <c r="G29">
-        <v>459</v>
+        <v>115</v>
       </c>
       <c r="H29">
-        <v>218</v>
+        <f t="shared" si="0"/>
+        <v>1.1057692307692308</v>
       </c>
       <c r="I29">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="2:9">
+      <c r="J29">
+        <v>459</v>
+      </c>
+      <c r="K29">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17">
       <c r="B30" t="s">
         <v>14</v>
       </c>
@@ -2486,7 +4025,7 @@
         <v>15</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -2495,16 +4034,23 @@
         <v>105.9</v>
       </c>
       <c r="G30">
-        <v>499</v>
+        <v>102</v>
       </c>
       <c r="H30">
-        <v>212</v>
+        <f t="shared" si="0"/>
+        <v>0.98076923076923073</v>
       </c>
       <c r="I30">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="2:9">
+      <c r="J30">
+        <v>499</v>
+      </c>
+      <c r="K30">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17">
       <c r="B31" t="s">
         <v>14</v>
       </c>
@@ -2512,7 +4058,7 @@
         <v>16</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
@@ -2521,16 +4067,23 @@
         <v>105.7</v>
       </c>
       <c r="G31">
-        <v>545</v>
+        <v>118</v>
       </c>
       <c r="H31">
-        <v>194</v>
+        <f t="shared" si="0"/>
+        <v>21.851851851851851</v>
       </c>
       <c r="I31">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="2:9">
+      <c r="J31">
+        <v>545</v>
+      </c>
+      <c r="K31">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17">
       <c r="B32" t="s">
         <v>14</v>
       </c>
@@ -2538,7 +4091,7 @@
         <v>16</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E32" t="s">
         <v>7</v>
@@ -2547,16 +4100,23 @@
         <v>147.4</v>
       </c>
       <c r="G32">
-        <v>700</v>
+        <v>187</v>
       </c>
       <c r="H32">
-        <v>211</v>
+        <f t="shared" si="0"/>
+        <v>34.629629629629626</v>
       </c>
       <c r="I32">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="33" spans="2:9">
+      <c r="J32">
+        <v>700</v>
+      </c>
+      <c r="K32">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13">
       <c r="B33" t="s">
         <v>14</v>
       </c>
@@ -2564,7 +4124,7 @@
         <v>16</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>5.4</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
@@ -2573,16 +4133,23 @@
         <v>158</v>
       </c>
       <c r="G33">
-        <v>678</v>
+        <v>178</v>
       </c>
       <c r="H33">
-        <v>233</v>
+        <f t="shared" si="0"/>
+        <v>32.962962962962962</v>
       </c>
       <c r="I33">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="2:9">
+      <c r="J33">
+        <v>678</v>
+      </c>
+      <c r="K33">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13">
       <c r="B34" t="s">
         <v>14</v>
       </c>
@@ -2590,7 +4157,7 @@
         <v>16</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E34" t="s">
         <v>6</v>
@@ -2599,16 +4166,23 @@
         <v>93.8</v>
       </c>
       <c r="G34">
-        <v>484</v>
+        <v>112</v>
       </c>
       <c r="H34">
-        <v>194</v>
+        <f t="shared" si="0"/>
+        <v>14.177215189873417</v>
       </c>
       <c r="I34">
         <v>14.9</v>
       </c>
-    </row>
-    <row r="35" spans="2:9">
+      <c r="J34">
+        <v>484</v>
+      </c>
+      <c r="K34">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13">
       <c r="B35" t="s">
         <v>14</v>
       </c>
@@ -2616,7 +4190,7 @@
         <v>16</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E35" t="s">
         <v>7</v>
@@ -2625,16 +4199,23 @@
         <v>108.2</v>
       </c>
       <c r="G35">
-        <v>561</v>
+        <v>162</v>
       </c>
       <c r="H35">
-        <v>193</v>
+        <f t="shared" si="0"/>
+        <v>20.50632911392405</v>
       </c>
       <c r="I35">
         <v>22.5</v>
       </c>
-    </row>
-    <row r="36" spans="2:9">
+      <c r="J35">
+        <v>561</v>
+      </c>
+      <c r="K35">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13">
       <c r="B36" t="s">
         <v>14</v>
       </c>
@@ -2642,7 +4223,7 @@
         <v>16</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>7.9</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
@@ -2651,16 +4232,23 @@
         <v>109.9</v>
       </c>
       <c r="G36">
-        <v>563</v>
+        <v>194</v>
       </c>
       <c r="H36">
-        <v>195</v>
+        <f t="shared" si="0"/>
+        <v>24.556962025316455</v>
       </c>
       <c r="I36">
         <v>17.3</v>
       </c>
-    </row>
-    <row r="37" spans="2:9">
+      <c r="J36">
+        <v>563</v>
+      </c>
+      <c r="K36">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13">
       <c r="B37" t="s">
         <v>14</v>
       </c>
@@ -2668,7 +4256,7 @@
         <v>16</v>
       </c>
       <c r="D37">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E37" t="s">
         <v>6</v>
@@ -2677,16 +4265,23 @@
         <v>68.5</v>
       </c>
       <c r="G37">
-        <v>410</v>
+        <v>181</v>
       </c>
       <c r="H37">
-        <v>167</v>
+        <f t="shared" si="0"/>
+        <v>1.7403846153846154</v>
       </c>
       <c r="I37">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="2:9">
+      <c r="J37">
+        <v>410</v>
+      </c>
+      <c r="K37">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13">
       <c r="B38" t="s">
         <v>14</v>
       </c>
@@ -2694,7 +4289,7 @@
         <v>16</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E38" t="s">
         <v>7</v>
@@ -2703,16 +4298,23 @@
         <v>104.5</v>
       </c>
       <c r="G38">
-        <v>461</v>
+        <v>207</v>
       </c>
       <c r="H38">
-        <v>227</v>
+        <f t="shared" si="0"/>
+        <v>1.9903846153846154</v>
       </c>
       <c r="I38">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="39" spans="2:9">
+      <c r="J38">
+        <v>461</v>
+      </c>
+      <c r="K38">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13">
       <c r="B39" t="s">
         <v>14</v>
       </c>
@@ -2720,7 +4322,7 @@
         <v>16</v>
       </c>
       <c r="D39">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="E39" t="s">
         <v>8</v>
@@ -2729,13 +4331,158 @@
         <v>104.2</v>
       </c>
       <c r="G39">
-        <v>467</v>
+        <v>200</v>
       </c>
       <c r="H39">
-        <v>223</v>
+        <f t="shared" si="0"/>
+        <v>1.9230769230769231</v>
       </c>
       <c r="I39">
         <v>16.7</v>
+      </c>
+      <c r="J39">
+        <v>467</v>
+      </c>
+      <c r="K39">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13">
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40">
+        <v>12.608333333333334</v>
+      </c>
+      <c r="I40">
+        <v>9.125</v>
+      </c>
+      <c r="J40">
+        <v>201</v>
+      </c>
+      <c r="L40">
+        <v>2.4</v>
+      </c>
+      <c r="M40">
+        <v>2053.2841812839974</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13">
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41">
+        <v>17.516666666666666</v>
+      </c>
+      <c r="I41">
+        <v>12.941666666666668</v>
+      </c>
+      <c r="J41">
+        <v>267.16666666666669</v>
+      </c>
+      <c r="L41">
+        <v>3</v>
+      </c>
+      <c r="M41">
+        <v>2666.9280374251107</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13">
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42">
+        <v>19.083333333333332</v>
+      </c>
+      <c r="I42">
+        <v>14.708333333333334</v>
+      </c>
+      <c r="J42">
+        <v>244.91666666666666</v>
+      </c>
+      <c r="L42">
+        <v>3.3</v>
+      </c>
+      <c r="M42">
+        <v>2965.1934863256661</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13">
+      <c r="B43" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" t="s">
+        <v>26</v>
+      </c>
+      <c r="H43">
+        <v>28.158333333333331</v>
+      </c>
+      <c r="I43">
+        <v>22.491666666666664</v>
+      </c>
+      <c r="J43">
+        <v>398.16666666666669</v>
+      </c>
+      <c r="L43">
+        <v>4.2</v>
+      </c>
+      <c r="M43">
+        <v>4872.3193140456788</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13">
+      <c r="B44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H44">
+        <v>38.43333333333333</v>
+      </c>
+      <c r="I44">
+        <v>28.175000000000001</v>
+      </c>
+      <c r="J44">
+        <v>437.75</v>
+      </c>
+      <c r="L44">
+        <v>5</v>
+      </c>
+      <c r="M44">
+        <v>5012.0274073398868</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13">
+      <c r="B45" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="4">
+        <v>47.358333333333327</v>
+      </c>
+      <c r="I45">
+        <v>31.183333333333337</v>
+      </c>
+      <c r="J45">
+        <v>434.5</v>
+      </c>
+      <c r="L45">
+        <v>5.3</v>
+      </c>
+      <c r="M45">
+        <v>5640.0645645995637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>